<commit_message>
trying new methods of scheduling requests
</commit_message>
<xml_diff>
--- a/CourseReqsParsed1.xlsx
+++ b/CourseReqsParsed1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Grace/Desktop/SENIOR PROJ/scheduling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F354B0-7345-1A41-A14F-EDAC8F5FB329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12F8AA0-3CFD-B44C-BCA5-5EDA53F3A537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1760" yWindow="760" windowWidth="27640" windowHeight="16600" activeTab="1" xr2:uid="{660C6E79-7610-B243-80E1-D564AB1DE7CD}"/>
   </bookViews>
@@ -17,6 +17,9 @@
     <sheet name="Classes" sheetId="3" r:id="rId2"/>
     <sheet name="Gr12" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Classes!$A$1:$C$21</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6304" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6322" uniqueCount="349">
   <si>
     <t>AGES</t>
   </si>
@@ -1048,9 +1051,6 @@
     <t>French 5 and 5H</t>
   </si>
   <si>
-    <t>French 4 </t>
-  </si>
-  <si>
     <t>Chinese 5 and 5H</t>
   </si>
   <si>
@@ -1070,6 +1070,24 @@
   </si>
   <si>
     <t>U7</t>
+  </si>
+  <si>
+    <t>U0.5</t>
+  </si>
+  <si>
+    <t>U8.5</t>
+  </si>
+  <si>
+    <t>U1.5</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t># Sections</t>
   </si>
 </sst>
 </file>
@@ -1079,7 +1097,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1105,6 +1123,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1126,11 +1151,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1467,8 +1493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DDB85B7-6B3D-0A4C-BFF3-CA2FF8D2CAF0}">
   <dimension ref="A1:H1030"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="A858" workbookViewId="0">
+      <selection activeCell="B748" sqref="B748"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11392,7 +11418,7 @@
         <v>89100</v>
       </c>
       <c r="B368" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C368" t="s">
         <v>228</v>
@@ -11419,7 +11445,7 @@
         <v>89067</v>
       </c>
       <c r="B369" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C369" t="s">
         <v>229</v>
@@ -11446,7 +11472,7 @@
         <v>89101</v>
       </c>
       <c r="B370" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C370" t="s">
         <v>229</v>
@@ -11473,7 +11499,7 @@
         <v>89064</v>
       </c>
       <c r="B371" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C371" t="s">
         <v>229</v>
@@ -11500,7 +11526,7 @@
         <v>89071</v>
       </c>
       <c r="B372" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C372" t="s">
         <v>229</v>
@@ -11527,7 +11553,7 @@
         <v>89056</v>
       </c>
       <c r="B373" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C373" t="s">
         <v>229</v>
@@ -11554,7 +11580,7 @@
         <v>89076</v>
       </c>
       <c r="B374" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C374" t="s">
         <v>229</v>
@@ -11581,7 +11607,7 @@
         <v>89057</v>
       </c>
       <c r="B375" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C375" t="s">
         <v>229</v>
@@ -11608,7 +11634,7 @@
         <v>89103</v>
       </c>
       <c r="B376" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C376" t="s">
         <v>229</v>
@@ -11635,7 +11661,7 @@
         <v>89072</v>
       </c>
       <c r="B377" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C377" t="s">
         <v>229</v>
@@ -11662,7 +11688,7 @@
         <v>89055</v>
       </c>
       <c r="B378" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C378" t="s">
         <v>229</v>
@@ -22327,7 +22353,7 @@
         <v>88566</v>
       </c>
       <c r="B773" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C773" t="s">
         <v>277</v>
@@ -22354,7 +22380,7 @@
         <v>89047</v>
       </c>
       <c r="B774" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C774" t="s">
         <v>277</v>
@@ -22381,7 +22407,7 @@
         <v>88594</v>
       </c>
       <c r="B775" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C775" t="s">
         <v>278</v>
@@ -22408,7 +22434,7 @@
         <v>88589</v>
       </c>
       <c r="B776" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C776" t="s">
         <v>278</v>
@@ -22435,7 +22461,7 @@
         <v>88552</v>
       </c>
       <c r="B777" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C777" t="s">
         <v>278</v>
@@ -22462,7 +22488,7 @@
         <v>88577</v>
       </c>
       <c r="B778" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C778" t="s">
         <v>278</v>
@@ -22489,7 +22515,7 @@
         <v>88562</v>
       </c>
       <c r="B779" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C779" t="s">
         <v>278</v>
@@ -22516,7 +22542,7 @@
         <v>89093</v>
       </c>
       <c r="B780" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C780" t="s">
         <v>279</v>
@@ -22543,7 +22569,7 @@
         <v>89084</v>
       </c>
       <c r="B781" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C781" t="s">
         <v>279</v>
@@ -22570,7 +22596,7 @@
         <v>89108</v>
       </c>
       <c r="B782" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C782" t="s">
         <v>279</v>
@@ -22597,7 +22623,7 @@
         <v>89074</v>
       </c>
       <c r="B783" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C783" t="s">
         <v>279</v>
@@ -22624,7 +22650,7 @@
         <v>89063</v>
       </c>
       <c r="B784" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C784" t="s">
         <v>279</v>
@@ -22651,7 +22677,7 @@
         <v>89082</v>
       </c>
       <c r="B785" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C785" t="s">
         <v>279</v>
@@ -29297,191 +29323,390 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9514B0BF-B51B-2446-AC8A-D06FAE1D5B91}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>207</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>215</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B15" t="s">
+        <v>343</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>230</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="B18" t="s">
+        <v>342</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="B19" t="s">
+        <v>341</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>242</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="B28" t="s">
+        <v>343</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>280</v>
+      </c>
+      <c r="B30" t="s">
+        <v>338</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>300</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>304</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B36" t="s">
+        <v>344</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>208</v>
+      </c>
+      <c r="B37" t="s">
+        <v>345</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="B38" t="s">
+        <v>341</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>308</v>
+      </c>
+      <c r="B39" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="B10" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="B11" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="B15" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>280</v>
-      </c>
-      <c r="B17" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="B20" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>208</v>
-      </c>
-      <c r="B21" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="B22" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>308</v>
-      </c>
-      <c r="B23" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="C39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>310</v>
       </c>
-      <c r="B24" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="3"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="3"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="3"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="3"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="3"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="3"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="3"/>
+      <c r="B40" t="s">
+        <v>337</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B32">
-    <sortCondition ref="A1:A32"/>
+  <autoFilter ref="A1:C21" xr:uid="{9514B0BF-B51B-2446-AC8A-D06FAE1D5B91}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C21">
+      <sortCondition ref="A1:A21"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B22">
+    <sortCondition ref="A2:A22"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>